<commit_message>
app10.py is latest version
</commit_message>
<xml_diff>
--- a/MockTB.xlsx
+++ b/MockTB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CallumMatchett\python\streamlit\div7a\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C90AF95-8469-4A74-BECF-C9E4E8996481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94307D78-6EE8-40CC-9637-43D24B3F0990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="1170" windowWidth="28410" windowHeight="10290" xr2:uid="{EA90E3A0-85DA-4522-BC8D-339C038AE014}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38400" windowHeight="14280" xr2:uid="{EA90E3A0-85DA-4522-BC8D-339C038AE014}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="47">
   <si>
     <t>AccountName</t>
   </si>
   <si>
-    <t>Office Equipment</t>
-  </si>
-  <si>
     <t>SourceAccountType</t>
   </si>
   <si>
@@ -71,63 +68,12 @@
     <t>Cash and Bank Balances</t>
   </si>
   <si>
-    <t>ANZ Bank Account</t>
-  </si>
-  <si>
     <t>NULL</t>
   </si>
   <si>
-    <t>BF Westpac Bank Account</t>
-  </si>
-  <si>
-    <t>Business Bank Account</t>
-  </si>
-  <si>
-    <t>Business Savings Account</t>
-  </si>
-  <si>
-    <t>Cash on Hand</t>
-  </si>
-  <si>
-    <t>CBA Bank Account</t>
-  </si>
-  <si>
-    <t>Chase Bank</t>
-  </si>
-  <si>
-    <t>NAB Bank Account</t>
-  </si>
-  <si>
-    <t>NZD ANZ Bank</t>
-  </si>
-  <si>
-    <t>Petty Cash</t>
-  </si>
-  <si>
-    <t>Petty Cash - Staff Amenities</t>
-  </si>
-  <si>
-    <t>SKK Bank Account</t>
-  </si>
-  <si>
-    <t>Westpac Bank</t>
-  </si>
-  <si>
-    <t>Westpac Bank Account</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
-    <t>OPENING Beef stock</t>
-  </si>
-  <si>
-    <t>Stock on Hand</t>
-  </si>
-  <si>
-    <t>Stock-on-Hand</t>
-  </si>
-  <si>
     <t>Other Assets</t>
   </si>
   <si>
@@ -137,108 +83,21 @@
     <t>Trade Receivables</t>
   </si>
   <si>
-    <t>Accounts Receivable</t>
-  </si>
-  <si>
-    <t>Trade Debtors</t>
-  </si>
-  <si>
-    <t>F05 Trade Debtors</t>
-  </si>
-  <si>
-    <t>Prepayments</t>
-  </si>
-  <si>
-    <t>Non-current Assets</t>
-  </si>
-  <si>
     <t>Intangibles</t>
   </si>
   <si>
-    <t>Borrowing Cost</t>
-  </si>
-  <si>
-    <t>Plant &amp; Equipment</t>
-  </si>
-  <si>
-    <t>Building - 67 Church St</t>
-  </si>
-  <si>
-    <t>Less Accumulated Depreciation on Motor Vehicles</t>
-  </si>
-  <si>
-    <t>Less Accumulated Depreciation on Office Equipment</t>
-  </si>
-  <si>
-    <t>Motor Vehicles</t>
-  </si>
-  <si>
-    <t>Fixed Assets Reconciliation</t>
-  </si>
-  <si>
-    <t>G10 Fixed Assets Rec</t>
-  </si>
-  <si>
     <t>Liabilities</t>
   </si>
   <si>
     <t>Current Liabilities</t>
   </si>
   <si>
-    <t>Credit Cards and Overdrafts</t>
-  </si>
-  <si>
-    <t>Wpc - Credit Card</t>
-  </si>
-  <si>
-    <t>GST Payable</t>
-  </si>
-  <si>
-    <t>GST</t>
-  </si>
-  <si>
-    <t>Income Tax Payable</t>
-  </si>
-  <si>
-    <t>Other Payables</t>
-  </si>
-  <si>
-    <t>PAYG Withholdings Payable</t>
-  </si>
-  <si>
-    <t>Superannuation Payable</t>
-  </si>
-  <si>
-    <t>Provisions</t>
-  </si>
-  <si>
-    <t>Provision for LSL</t>
-  </si>
-  <si>
-    <t>Trade Payables</t>
-  </si>
-  <si>
-    <t>Accounts Payable</t>
-  </si>
-  <si>
-    <t>Trade Creditors</t>
-  </si>
-  <si>
     <t>Non-current Liabilities</t>
   </si>
   <si>
     <t>Borrowings</t>
   </si>
   <si>
-    <t>CBA Loan - Building</t>
-  </si>
-  <si>
-    <t>Less: Unexpired Interest Tesla - Current</t>
-  </si>
-  <si>
-    <t>Less: Unexpired Interest Tesla - Non-Current</t>
-  </si>
-  <si>
     <t>Tesla Loan - Current</t>
   </si>
   <si>
@@ -249,14 +108,91 @@
   </si>
   <si>
     <t>Division 7A</t>
+  </si>
+  <si>
+    <t>Payroll</t>
+  </si>
+  <si>
+    <t>Associate  Debt</t>
+  </si>
+  <si>
+    <t>Current Account - J Smith</t>
+  </si>
+  <si>
+    <t>Short Term Advance Account</t>
+  </si>
+  <si>
+    <t>Business Development Loan</t>
+  </si>
+  <si>
+    <t>Temporary Funding Account</t>
+  </si>
+  <si>
+    <t>Working Capital Advance</t>
+  </si>
+  <si>
+    <t>Special Purpose Vehicle Account</t>
+  </si>
+  <si>
+    <t>Investment Holdings Account</t>
+  </si>
+  <si>
+    <t>Management Account - Personal</t>
+  </si>
+  <si>
+    <t>Consulting Fees Receivable</t>
+  </si>
+  <si>
+    <t>Private Company Advance</t>
+  </si>
+  <si>
+    <t>Distribution Account Payable</t>
+  </si>
+  <si>
+    <t>Entity B Current Account</t>
+  </si>
+  <si>
+    <t>Corporate Development Fund</t>
+  </si>
+  <si>
+    <t>Special Drawing Rights</t>
+  </si>
+  <si>
+    <t>Trust Beneficiary Account</t>
+  </si>
+  <si>
+    <t>Business Owner Advance</t>
+  </si>
+  <si>
+    <t>Internal Funding Account</t>
+  </si>
+  <si>
+    <t>Personal Transactions Clearing</t>
+  </si>
+  <si>
+    <t>Management Participation Account</t>
+  </si>
+  <si>
+    <t>Associated Entity Balance</t>
+  </si>
+  <si>
+    <t>Car Loan - Non-Current</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -284,8 +220,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EA7D87A-CE41-4647-AE05-D437DEC7F586}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,1018 +576,680 @@
     <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F2">
-        <v>-750</v>
+        <v>-50243</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F3">
-        <v>3151800.35</v>
+        <v>500</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>-15944</v>
+        <v>-348525.16</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>9400</v>
+        <v>-348525.16</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>512</v>
+        <v>-348525.16</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>276279.81</v>
+        <v>-348525.16</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>504482.6</v>
+        <v>-348525.16</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>-46204.07</v>
+        <v>-348525.16</v>
       </c>
       <c r="G9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>45645.01</v>
+        <v>-348525.16</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F11">
-        <v>1200</v>
+        <v>500</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F12">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="G12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F13">
-        <v>6424.78</v>
+        <v>500</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F14">
-        <v>56642.86</v>
+        <v>500</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F15">
-        <v>-4481.6400000000003</v>
+        <v>500</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F16">
-        <v>100000</v>
+        <v>500</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F17">
-        <v>-250</v>
+        <v>500</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F18">
-        <v>852729.54</v>
+        <v>500</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F19">
-        <v>-348525.16</v>
+        <v>500</v>
       </c>
       <c r="G19" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F20">
-        <v>1951711.98</v>
+        <v>500</v>
       </c>
       <c r="G20" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="H20" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F21">
-        <v>3640</v>
+        <v>500</v>
       </c>
       <c r="G21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F22">
-        <v>-1200</v>
+        <v>500</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F23">
-        <v>340318.09</v>
+        <v>500</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="B24" t="s">
-        <v>37</v>
-      </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24">
-        <v>-25050</v>
+        <v>-348525.16</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H24" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F25">
-        <v>-64031.88</v>
+        <v>17644</v>
       </c>
       <c r="G25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F26">
-        <v>139187</v>
+        <v>-50243</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="H26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>70010.460000000006</v>
-      </c>
-      <c r="G27" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" t="s">
-        <v>50</v>
-      </c>
-      <c r="E28">
-        <v>-1</v>
-      </c>
-      <c r="F28">
-        <v>-10494</v>
-      </c>
-      <c r="G28" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29">
-        <v>-1</v>
-      </c>
-      <c r="F29">
-        <v>-245468.61</v>
-      </c>
-      <c r="G29" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30">
-        <v>-1</v>
-      </c>
-      <c r="F30">
-        <v>-505693.6</v>
-      </c>
-      <c r="G30" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31">
-        <v>-1</v>
-      </c>
-      <c r="F31">
-        <v>-53436</v>
-      </c>
-      <c r="G31" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" t="s">
-        <v>54</v>
-      </c>
-      <c r="D32" t="s">
-        <v>56</v>
-      </c>
-      <c r="E32">
-        <v>-1</v>
-      </c>
-      <c r="F32">
-        <v>-17771.8</v>
-      </c>
-      <c r="G32" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" t="s">
-        <v>57</v>
-      </c>
-      <c r="D33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E33">
-        <v>-1</v>
-      </c>
-      <c r="F33">
-        <v>-1000</v>
-      </c>
-      <c r="G33" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>47</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
-      <c r="E34">
-        <v>-1</v>
-      </c>
-      <c r="F34">
-        <v>-254906.66</v>
-      </c>
-      <c r="G34" t="s">
-        <v>61</v>
-      </c>
-      <c r="H34" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D35" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35">
-        <v>-1</v>
-      </c>
-      <c r="F35">
-        <v>-306506.56</v>
-      </c>
-      <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36">
-        <v>-1</v>
-      </c>
-      <c r="F36">
-        <v>3792.86</v>
-      </c>
-      <c r="G36" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E37">
-        <v>-1</v>
-      </c>
-      <c r="F37">
-        <v>5753.78</v>
-      </c>
-      <c r="G37" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D38" t="s">
-        <v>67</v>
-      </c>
-      <c r="E38">
-        <v>-1</v>
-      </c>
-      <c r="F38">
-        <v>17644</v>
-      </c>
-      <c r="G38" t="s">
-        <v>12</v>
-      </c>
-      <c r="H38" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" t="s">
-        <v>63</v>
-      </c>
-      <c r="D39" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39">
-        <v>-1</v>
-      </c>
-      <c r="F39">
-        <v>-50243</v>
-      </c>
-      <c r="G39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>